<commit_message>
Adding loginData file new
</commit_message>
<xml_diff>
--- a/src/test/java/com/inetBankingV4/testData/LoginData.xlsx
+++ b/src/test/java/com/inetBankingV4/testData/LoginData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsrin\workspace\InetBankingV3\src\test\java\com\inetBanking\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsrin\workspace\Guru99Project\src\test\java\com\guru99\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED09B02-C0DD-4CE1-B8DA-771FDB2A3CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED97918-977B-42A6-82F1-E53D081E7DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{744AAAF0-8BCA-4986-9F2D-DB4FC912F9F0}"/>
+    <workbookView xWindow="900" yWindow="1890" windowWidth="16845" windowHeight="7830" xr2:uid="{744AAAF0-8BCA-4986-9F2D-DB4FC912F9F0}"/>
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
@@ -33,25 +33,10 @@
     <t>password</t>
   </si>
   <si>
-    <t>mngr140789</t>
+    <t>mngr353180</t>
   </si>
   <si>
-    <t>AeUdYdf</t>
-  </si>
-  <si>
-    <t>mngr412356</t>
-  </si>
-  <si>
-    <t>mngr318762</t>
-  </si>
-  <si>
-    <t>UmejUru</t>
-  </si>
-  <si>
-    <t>mngr347851</t>
-  </si>
-  <si>
-    <t>tUpeqUv</t>
+    <t>nerynYt</t>
   </si>
 </sst>
 </file>
@@ -436,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3039F9A8-3D97-41FF-8FEF-D3BB52406438}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,10 +442,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -468,30 +453,6 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>